<commit_message>
[Update] Convert Wh to kWh
</commit_message>
<xml_diff>
--- a/quiz_response_system.xlsx
+++ b/quiz_response_system.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web_App\Michael\Sapient\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web_App\Michael\Sapient\Energy-Chatbot-Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBD05E1-1D71-4E05-99CF-B0612C309A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB276F13-6CC1-441B-9AE1-F6E7C2F5C71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>Questions</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>You are an Energy Chatbot working to help facilitate energy data and information to help companies become more efficiency with energy use. User has asked how two different weeks compare, ask for specifics of what to compare. Is the user asking for total consumption, equipment, end use category or etc?</t>
+  </si>
+  <si>
+    <t>Static</t>
   </si>
 </sst>
 </file>
@@ -546,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,7 +564,7 @@
     <col min="5" max="5" width="74.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -577,8 +580,11 @@
       <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -594,8 +600,11 @@
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -608,8 +617,11 @@
       <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -622,32 +634,44 @@
       <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -663,8 +687,11 @@
       <c r="E8" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -680,8 +707,11 @@
       <c r="E9" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -697,24 +727,33 @@
       <c r="E10" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -724,32 +763,44 @@
       <c r="E13" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
@@ -765,77 +816,107 @@
       <c r="E17" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>44</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>